<commit_message>
Fix to deal with multiple lines per interview/species
</commit_message>
<xml_diff>
--- a/R/HMRFS/MRIP_Ifiles_HI/HMRFS catch.xlsx
+++ b/R/HMRFS/MRIP_Ifiles_HI/HMRFS catch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toby/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toby/Documents/GitHub/MHI_Bottomfish_2023/R/HMRFS/MRIP_Ifiles_HI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4C8E5C-D070-2444-9286-3E2BA49AC160}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57833B80-FF5F-1F48-9834-A9430A2FE09E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{F0835D66-C3C9-A940-B09B-9B4D038C55CA}"/>
+    <workbookView xWindow="1040" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{F0835D66-C3C9-A940-B09B-9B4D038C55CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -462,10 +462,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A31AAAF-CF5B-9B4D-B312-EE268438E283}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:N125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -514,7 +515,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" hidden="1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -558,7 +559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" hidden="1">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -602,7 +603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" hidden="1">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -646,7 +647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" hidden="1">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
@@ -690,7 +691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" hidden="1">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -734,7 +735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" hidden="1">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -778,7 +779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" hidden="1">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -822,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" hidden="1">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -866,7 +867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" hidden="1">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -910,7 +911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" hidden="1">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -954,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" hidden="1">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -998,7 +999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" hidden="1">
       <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
@@ -1042,7 +1043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" hidden="1">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
@@ -1086,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" hidden="1">
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
@@ -1130,7 +1131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" hidden="1">
       <c r="A16" s="2" t="s">
         <v>10</v>
       </c>
@@ -1174,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" hidden="1">
       <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
@@ -1218,7 +1219,7 @@
         <v>0.41</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" hidden="1">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
@@ -1262,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" hidden="1">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
@@ -1306,7 +1307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" hidden="1">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -1350,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" hidden="1">
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
@@ -1394,7 +1395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" hidden="1">
       <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
@@ -1438,7 +1439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" hidden="1">
       <c r="A23" s="2" t="s">
         <v>10</v>
       </c>
@@ -1482,7 +1483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" hidden="1">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" hidden="1">
       <c r="A25" s="2" t="s">
         <v>10</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" hidden="1">
       <c r="A26" s="2" t="s">
         <v>10</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" hidden="1">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -1658,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" hidden="1">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -1702,7 +1703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" hidden="1">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" hidden="1">
       <c r="A30" s="2" t="s">
         <v>10</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" hidden="1">
       <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
@@ -1834,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" hidden="1">
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
@@ -1878,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" hidden="1">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
@@ -1922,7 +1923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" hidden="1">
       <c r="A34" s="2" t="s">
         <v>10</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" hidden="1">
       <c r="A35" s="2" t="s">
         <v>10</v>
       </c>
@@ -2010,7 +2011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" hidden="1">
       <c r="A36" s="2" t="s">
         <v>15</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" hidden="1">
       <c r="A37" s="2" t="s">
         <v>10</v>
       </c>
@@ -2098,7 +2099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" hidden="1">
       <c r="A38" s="2" t="s">
         <v>10</v>
       </c>
@@ -2142,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:14">
+    <row r="39" spans="1:14" hidden="1">
       <c r="A39" s="2" t="s">
         <v>10</v>
       </c>
@@ -2186,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:14">
+    <row r="40" spans="1:14" hidden="1">
       <c r="A40" s="2" t="s">
         <v>10</v>
       </c>
@@ -2230,7 +2231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" hidden="1">
       <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
@@ -2274,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" hidden="1">
       <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
@@ -2318,7 +2319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" hidden="1">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -2362,7 +2363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" hidden="1">
       <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" hidden="1">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -2450,7 +2451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" hidden="1">
       <c r="A46" s="2" t="s">
         <v>10</v>
       </c>
@@ -2494,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" hidden="1">
       <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
@@ -2538,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" hidden="1">
       <c r="A48" s="2" t="s">
         <v>10</v>
       </c>
@@ -2582,7 +2583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14">
+    <row r="49" spans="1:14" hidden="1">
       <c r="A49" s="2" t="s">
         <v>10</v>
       </c>
@@ -2626,7 +2627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:14">
+    <row r="50" spans="1:14" hidden="1">
       <c r="A50" s="2" t="s">
         <v>10</v>
       </c>
@@ -2670,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:14">
+    <row r="51" spans="1:14" hidden="1">
       <c r="A51" s="2" t="s">
         <v>10</v>
       </c>
@@ -2714,7 +2715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:14">
+    <row r="52" spans="1:14" hidden="1">
       <c r="A52" s="2" t="s">
         <v>10</v>
       </c>
@@ -2758,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:14">
+    <row r="53" spans="1:14" hidden="1">
       <c r="A53" s="2" t="s">
         <v>10</v>
       </c>
@@ -2802,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:14">
+    <row r="54" spans="1:14" hidden="1">
       <c r="A54" s="2" t="s">
         <v>15</v>
       </c>
@@ -3726,7 +3727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:14">
+    <row r="75" spans="1:14" hidden="1">
       <c r="A75" s="2" t="s">
         <v>10</v>
       </c>
@@ -3770,7 +3771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:14">
+    <row r="76" spans="1:14" hidden="1">
       <c r="A76" s="2" t="s">
         <v>10</v>
       </c>
@@ -3814,7 +3815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:14">
+    <row r="77" spans="1:14" hidden="1">
       <c r="A77" s="2" t="s">
         <v>10</v>
       </c>
@@ -3858,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:14">
+    <row r="78" spans="1:14" hidden="1">
       <c r="A78" s="2" t="s">
         <v>10</v>
       </c>
@@ -3902,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:14">
+    <row r="79" spans="1:14" hidden="1">
       <c r="A79" s="2" t="s">
         <v>10</v>
       </c>
@@ -3946,7 +3947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:14">
+    <row r="80" spans="1:14" hidden="1">
       <c r="A80" s="2" t="s">
         <v>10</v>
       </c>
@@ -3990,7 +3991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:14">
+    <row r="81" spans="1:14" hidden="1">
       <c r="A81" s="2" t="s">
         <v>10</v>
       </c>
@@ -4034,7 +4035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:14">
+    <row r="82" spans="1:14" hidden="1">
       <c r="A82" s="2" t="s">
         <v>10</v>
       </c>
@@ -4078,7 +4079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:14">
+    <row r="83" spans="1:14" hidden="1">
       <c r="A83" s="2" t="s">
         <v>10</v>
       </c>
@@ -4122,7 +4123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:14">
+    <row r="84" spans="1:14" hidden="1">
       <c r="A84" s="2" t="s">
         <v>10</v>
       </c>
@@ -4166,7 +4167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:14">
+    <row r="85" spans="1:14" hidden="1">
       <c r="A85" s="2" t="s">
         <v>10</v>
       </c>
@@ -4210,7 +4211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:14">
+    <row r="86" spans="1:14" hidden="1">
       <c r="A86" s="2" t="s">
         <v>10</v>
       </c>
@@ -4254,7 +4255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:14">
+    <row r="87" spans="1:14" hidden="1">
       <c r="A87" s="2" t="s">
         <v>10</v>
       </c>
@@ -4298,7 +4299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:14">
+    <row r="88" spans="1:14" hidden="1">
       <c r="A88" s="2" t="s">
         <v>10</v>
       </c>
@@ -4342,7 +4343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:14">
+    <row r="89" spans="1:14" hidden="1">
       <c r="A89" s="2" t="s">
         <v>10</v>
       </c>
@@ -4386,7 +4387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:14">
+    <row r="90" spans="1:14" hidden="1">
       <c r="A90" s="2" t="s">
         <v>10</v>
       </c>
@@ -4430,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:14">
+    <row r="91" spans="1:14" hidden="1">
       <c r="A91" s="2" t="s">
         <v>10</v>
       </c>
@@ -4474,7 +4475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:14">
+    <row r="92" spans="1:14" hidden="1">
       <c r="A92" s="2" t="s">
         <v>10</v>
       </c>
@@ -4518,7 +4519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
+    <row r="93" spans="1:14" hidden="1">
       <c r="A93" s="2" t="s">
         <v>15</v>
       </c>
@@ -4562,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
+    <row r="94" spans="1:14" hidden="1">
       <c r="A94" s="2" t="s">
         <v>10</v>
       </c>
@@ -4606,7 +4607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:14">
+    <row r="95" spans="1:14" hidden="1">
       <c r="A95" s="2" t="s">
         <v>10</v>
       </c>
@@ -4650,7 +4651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
+    <row r="96" spans="1:14" hidden="1">
       <c r="A96" s="2" t="s">
         <v>10</v>
       </c>
@@ -4694,7 +4695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
+    <row r="97" spans="1:14" hidden="1">
       <c r="A97" s="2" t="s">
         <v>10</v>
       </c>
@@ -4738,7 +4739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:14">
+    <row r="98" spans="1:14" hidden="1">
       <c r="A98" s="2" t="s">
         <v>10</v>
       </c>
@@ -4782,7 +4783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
+    <row r="99" spans="1:14" hidden="1">
       <c r="A99" s="2" t="s">
         <v>10</v>
       </c>
@@ -4826,7 +4827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:14">
+    <row r="100" spans="1:14" hidden="1">
       <c r="A100" s="2" t="s">
         <v>10</v>
       </c>
@@ -4870,7 +4871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:14" hidden="1">
       <c r="A101" s="2" t="s">
         <v>10</v>
       </c>
@@ -4914,7 +4915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:14">
+    <row r="102" spans="1:14" hidden="1">
       <c r="A102" s="2" t="s">
         <v>10</v>
       </c>
@@ -4958,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:14">
+    <row r="103" spans="1:14" hidden="1">
       <c r="A103" s="2" t="s">
         <v>10</v>
       </c>
@@ -5002,7 +5003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:14" hidden="1">
       <c r="A104" s="2" t="s">
         <v>10</v>
       </c>
@@ -5046,7 +5047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:14" hidden="1">
       <c r="A105" s="2" t="s">
         <v>10</v>
       </c>
@@ -5090,7 +5091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:14" hidden="1">
       <c r="A106" s="2" t="s">
         <v>10</v>
       </c>
@@ -5134,7 +5135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:14">
+    <row r="107" spans="1:14" hidden="1">
       <c r="A107" s="2" t="s">
         <v>10</v>
       </c>
@@ -5178,7 +5179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:14">
+    <row r="108" spans="1:14" hidden="1">
       <c r="A108" s="2" t="s">
         <v>15</v>
       </c>
@@ -5222,7 +5223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:14" hidden="1">
       <c r="A109" s="2" t="s">
         <v>10</v>
       </c>
@@ -5266,7 +5267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:14">
+    <row r="110" spans="1:14" hidden="1">
       <c r="A110" s="2" t="s">
         <v>10</v>
       </c>
@@ -5310,7 +5311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:14">
+    <row r="111" spans="1:14" hidden="1">
       <c r="A111" s="2" t="s">
         <v>10</v>
       </c>
@@ -5354,7 +5355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:14" hidden="1">
       <c r="A112" s="2" t="s">
         <v>10</v>
       </c>
@@ -5398,7 +5399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:14" hidden="1">
       <c r="A113" s="2" t="s">
         <v>10</v>
       </c>
@@ -5442,7 +5443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:14" hidden="1">
       <c r="A114" s="2" t="s">
         <v>10</v>
       </c>
@@ -5486,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:14" hidden="1">
       <c r="A115" s="2" t="s">
         <v>10</v>
       </c>
@@ -5530,7 +5531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:14" hidden="1">
       <c r="A116" s="2" t="s">
         <v>10</v>
       </c>
@@ -5574,7 +5575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:14" hidden="1">
       <c r="A117" s="2" t="s">
         <v>10</v>
       </c>
@@ -5618,7 +5619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:14" hidden="1">
       <c r="A118" s="2" t="s">
         <v>10</v>
       </c>
@@ -5662,7 +5663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:14">
+    <row r="119" spans="1:14" hidden="1">
       <c r="A119" s="2" t="s">
         <v>10</v>
       </c>
@@ -5706,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:14">
+    <row r="120" spans="1:14" hidden="1">
       <c r="A120" s="2" t="s">
         <v>10</v>
       </c>
@@ -5750,7 +5751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:14" hidden="1">
       <c r="A121" s="2" t="s">
         <v>10</v>
       </c>
@@ -5794,7 +5795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:14" hidden="1">
       <c r="A122" s="2" t="s">
         <v>10</v>
       </c>
@@ -5838,7 +5839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:14" hidden="1">
       <c r="A123" s="2" t="s">
         <v>10</v>
       </c>
@@ -5882,7 +5883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:14" hidden="1">
       <c r="A124" s="2" t="s">
         <v>10</v>
       </c>
@@ -5926,7 +5927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:14" hidden="1">
       <c r="A125" s="2" t="s">
         <v>15</v>
       </c>
@@ -5971,7 +5972,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N125" xr:uid="{36D5F977-24D3-F04D-B028-4860A4020BF7}"/>
+  <autoFilter ref="A1:N125" xr:uid="{36D5F977-24D3-F04D-B028-4860A4020BF7}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="PINK SNAPPER"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>